<commit_message>
updated HIV/TB model and param file
</commit_message>
<xml_diff>
--- a/model_outputs/euler_comparison_TBonly.xlsx
+++ b/model_outputs/euler_comparison_TBonly.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/github/epi_model_HIV_TB/model_outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28155743-17AB-6649-AE4F-1AD2D836066A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E40FA510-AB33-ED40-8D74-246CA69B5176}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="out" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="19" uniqueCount="10">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="35" uniqueCount="26">
   <si>
     <t>time</t>
   </si>
@@ -65,11 +67,62 @@
   <si>
     <t>total_pop</t>
   </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>iota</t>
+  </si>
+  <si>
+    <t>zeta</t>
+  </si>
+  <si>
+    <t>upsilon</t>
+  </si>
+  <si>
+    <t>kappa_t</t>
+  </si>
+  <si>
+    <t>alpha_in_t</t>
+  </si>
+  <si>
+    <t>varpi</t>
+  </si>
+  <si>
+    <t>omega</t>
+  </si>
+  <si>
+    <t>FOI</t>
+  </si>
+  <si>
+    <t>BIRTHS</t>
+  </si>
+  <si>
+    <t>total_out_t</t>
+  </si>
+  <si>
+    <t>prob age out</t>
+  </si>
+  <si>
+    <t>prob die</t>
+  </si>
+  <si>
+    <t>prob age out and die</t>
+  </si>
+  <si>
+    <t>Uninfected</t>
+  </si>
+  <si>
+    <t>Infected</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -206,7 +259,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,6 +451,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -559,10 +618,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -918,15 +980,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S62"/>
+  <dimension ref="A1:W62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -957,35 +1019,47 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1016,44 +1090,60 @@
       <c r="J2">
         <v>100000</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="5">
+        <f>B2+C2</f>
+        <v>38138.825324179998</v>
+      </c>
+      <c r="L2">
+        <f>I2+G2</f>
+        <v>17467.581998474401</v>
+      </c>
+      <c r="M2">
+        <f>(G2/J2)*Sheet1!$B$2</f>
+        <v>1.6135774218154075E-4</v>
+      </c>
+      <c r="N2">
+        <f>SUMPRODUCT(B2:I2,Sheet1!B13:I13)/12</f>
+        <v>304.78648881261068</v>
+      </c>
+      <c r="O2">
         <f>B2</f>
         <v>19069.412662089999</v>
       </c>
-      <c r="L2">
-        <f t="shared" ref="L2:R2" si="0">C2</f>
+      <c r="P2">
+        <f>C2</f>
         <v>19069.412662089999</v>
       </c>
-      <c r="M2">
-        <f t="shared" si="0"/>
+      <c r="Q2">
+        <f t="shared" ref="Q2:V2" si="0">D2</f>
         <v>14797.864225781799</v>
-      </c>
-      <c r="N2">
-        <f t="shared" si="0"/>
-        <v>14797.864225781799</v>
-      </c>
-      <c r="O2">
-        <f t="shared" si="0"/>
-        <v>14797.864225781799</v>
-      </c>
-      <c r="P2">
-        <f t="shared" si="0"/>
-        <v>2669.7177726926002</v>
-      </c>
-      <c r="Q2">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
       <c r="R2">
         <f t="shared" si="0"/>
         <v>14797.864225781799</v>
       </c>
       <c r="S2">
-        <f>SUM(K2:R2)</f>
+        <f t="shared" si="0"/>
+        <v>14797.864225781799</v>
+      </c>
+      <c r="T2">
+        <f t="shared" si="0"/>
+        <v>2669.7177726926002</v>
+      </c>
+      <c r="U2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <f t="shared" si="0"/>
+        <v>14797.864225781799</v>
+      </c>
+      <c r="W2">
+        <f>SUM(O2:V2)</f>
         <v>99999.999999999796</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>8.3333333333333301E-2</v>
       </c>
@@ -1084,8 +1174,52 @@
       <c r="J3">
         <v>100000</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K3" s="5">
+        <f t="shared" ref="K3:K62" si="1">B3+C3</f>
+        <v>38149.004283776398</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L62" si="2">I3+G3</f>
+        <v>19637.766860598822</v>
+      </c>
+      <c r="M3">
+        <f>(G3/J3)*Sheet1!$B$2</f>
+        <v>1.5811942428602959E-4</v>
+      </c>
+      <c r="O3">
+        <f>($N2*Sheet1!B11)+((Sheet1!B7/12)*(out!P2))</f>
+        <v>3294.9554304957546</v>
+      </c>
+      <c r="P3">
+        <f>$N2*Sheet1!C11</f>
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f>$N2*Sheet1!D11</f>
+        <v>92.873621158860914</v>
+      </c>
+      <c r="R3">
+        <f>$N2*Sheet1!E11</f>
+        <v>92.873621158860914</v>
+      </c>
+      <c r="S3">
+        <f>$N2*Sheet1!F11</f>
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <f>$N2*Sheet1!G11</f>
+        <v>2.3192599855870308</v>
+      </c>
+      <c r="U3">
+        <f>$N2*Sheet1!H11</f>
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <f>$N2*Sheet1!I11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0.16666666666666599</v>
       </c>
@@ -1116,8 +1250,20 @@
       <c r="J4">
         <v>100000</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K4" s="5">
+        <f t="shared" si="1"/>
+        <v>38158.876805909196</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="2"/>
+        <v>21425.991222060111</v>
+      </c>
+      <c r="M4">
+        <f>(G4/J4)*Sheet1!$B$2</f>
+        <v>1.5345425355876632E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.25</v>
       </c>
@@ -1148,8 +1294,20 @@
       <c r="J5">
         <v>100000</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K5" s="5">
+        <f t="shared" si="1"/>
+        <v>38168.378961812297</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>22898.015729406899</v>
+      </c>
+      <c r="M5">
+        <f>(G5/J5)*Sheet1!$B$2</f>
+        <v>1.4781987992727676E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.33333333333333298</v>
       </c>
@@ -1180,8 +1338,20 @@
       <c r="J6">
         <v>100000</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K6" s="5">
+        <f t="shared" si="1"/>
+        <v>38177.470625623879</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>24108.397500197942</v>
+      </c>
+      <c r="M6">
+        <f>(G6/J6)*Sheet1!$B$2</f>
+        <v>1.4156875976273529E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.41666666666666602</v>
       </c>
@@ -1212,8 +1382,20 @@
       <c r="J7">
         <v>100000</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K7" s="5">
+        <f t="shared" si="1"/>
+        <v>38186.129602593996</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>25102.384448714118</v>
+      </c>
+      <c r="M7">
+        <f>(G7/J7)*Sheet1!$B$2</f>
+        <v>1.3496983201094173E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.5</v>
       </c>
@@ -1244,8 +1426,21 @@
       <c r="J8">
         <v>100000</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K8" s="5">
+        <f t="shared" si="1"/>
+        <v>38194.347058076142</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>25917.495712430002</v>
+      </c>
+      <c r="M8">
+        <f>(G8/J8)*Sheet1!$B$2</f>
+        <v>1.2822603887217287E-4</v>
+      </c>
+      <c r="O8" s="4"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.58333333333333304</v>
       </c>
@@ -1276,8 +1471,20 @@
       <c r="J9">
         <v>100000</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K9" s="5">
+        <f t="shared" si="1"/>
+        <v>38202.123990207154</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>26584.834556949758</v>
+      </c>
+      <c r="M9">
+        <f>(G9/J9)*Sheet1!$B$2</f>
+        <v>1.2148836071036739E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.66666666666666596</v>
       </c>
@@ -1308,8 +1515,20 @@
       <c r="J10">
         <v>100000</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K10" s="5">
+        <f t="shared" si="1"/>
+        <v>38209.468479741248</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>27130.18642731099</v>
+      </c>
+      <c r="M10">
+        <f>(G10/J10)*Sheet1!$B$2</f>
+        <v>1.1486714531984489E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.75</v>
       </c>
@@ -1340,8 +1559,20 @@
       <c r="J11">
         <v>100000</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K11" s="5">
+        <f t="shared" si="1"/>
+        <v>38216.393673779014</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>27574.903340164128</v>
+      </c>
+      <c r="M11">
+        <f>(G11/J11)*Sheet1!$B$2</f>
+        <v>1.0844080540933174E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.83333333333333304</v>
       </c>
@@ -1372,8 +1603,20 @@
       <c r="J12">
         <v>100000</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K12" s="5">
+        <f t="shared" si="1"/>
+        <v>38222.916090010731</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>27936.67891071146</v>
+      </c>
+      <c r="M12">
+        <f>(G12/J12)*Sheet1!$B$2</f>
+        <v>1.0226326933613073E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0.91666666666666596</v>
       </c>
@@ -1404,8 +1647,20 @@
       <c r="J13">
         <v>100000</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K13" s="5">
+        <f t="shared" si="1"/>
+        <v>38229.054426438954</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="2"/>
+        <v>28230.16409609246</v>
+      </c>
+      <c r="M13">
+        <f>(G13/J13)*Sheet1!$B$2</f>
+        <v>9.6369538889364229E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1436,8 +1691,20 @@
       <c r="J14">
         <v>100000</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K14" s="5">
+        <f t="shared" si="1"/>
+        <v>38234.828653143362</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="2"/>
+        <v>28467.481924470729</v>
+      </c>
+      <c r="M14">
+        <f>(G14/J14)*Sheet1!$B$2</f>
+        <v>9.0780121848124277E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1.0833333333333299</v>
       </c>
@@ -1468,8 +1735,20 @@
       <c r="J15">
         <v>100000</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K15" s="5">
+        <f t="shared" si="1"/>
+        <v>38240.259292163559</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>28658.663346266771</v>
+      </c>
+      <c r="M15">
+        <f>(G15/J15)*Sheet1!$B$2</f>
+        <v>8.5504667188256154E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1.1666666666666601</v>
       </c>
@@ -1500,8 +1779,20 @@
       <c r="J16">
         <v>100000</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="5">
+        <f t="shared" si="1"/>
+        <v>38245.366917996842</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="2"/>
+        <v>28812.001930840081</v>
+      </c>
+      <c r="M16">
+        <f>(G16/J16)*Sheet1!$B$2</f>
+        <v>8.0544706371359212E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1.25</v>
       </c>
@@ -1532,8 +1823,20 @@
       <c r="J17">
         <v>100000</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="5">
+        <f t="shared" si="1"/>
+        <v>38250.17178010894</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>28934.351594436917</v>
+      </c>
+      <c r="M17">
+        <f>(G17/J17)*Sheet1!$B$2</f>
+        <v>7.5895851430675385E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1.3333333333333299</v>
       </c>
@@ -1564,8 +1867,20 @@
       <c r="J18">
         <v>100000</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18" s="5">
+        <f t="shared" si="1"/>
+        <v>38254.693536750114</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="2"/>
+        <v>29031.373158518891</v>
+      </c>
+      <c r="M18">
+        <f>(G18/J18)*Sheet1!$B$2</f>
+        <v>7.154949985705351E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1.4166666666666601</v>
       </c>
@@ -1596,8 +1911,20 @@
       <c r="J19">
         <v>100000</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19" s="5">
+        <f t="shared" si="1"/>
+        <v>38258.951077670936</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="2"/>
+        <v>29107.738248156282</v>
+      </c>
+      <c r="M19">
+        <f>(G19/J19)*Sheet1!$B$2</f>
+        <v>6.7494137702154666E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1.5</v>
       </c>
@@ -1628,8 +1955,20 @@
       <c r="J20">
         <v>100000</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20" s="5">
+        <f t="shared" si="1"/>
+        <v>38262.962404903679</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="2"/>
+        <v>29167.299354903</v>
+      </c>
+      <c r="M20">
+        <f>(G20/J20)*Sheet1!$B$2</f>
+        <v>6.3716356999255622E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1.5833333333333299</v>
       </c>
@@ -1660,8 +1999,20 @@
       <c r="J21">
         <v>100000</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21" s="5">
+        <f t="shared" si="1"/>
+        <v>38266.744565280031</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="2"/>
+        <v>29213.230472151045</v>
+      </c>
+      <c r="M21">
+        <f>(G21/J21)*Sheet1!$B$2</f>
+        <v>6.0201621224290639E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1.6666666666666601</v>
       </c>
@@ -1692,8 +2043,20 @@
       <c r="J22">
         <v>100000</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K22" s="5">
+        <f t="shared" si="1"/>
+        <v>38270.313618662803</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="2"/>
+        <v>29248.143880603595</v>
+      </c>
+      <c r="M22">
+        <f>(G22/J22)*Sheet1!$B$2</f>
+        <v>5.6934843008187902E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1.75</v>
       </c>
@@ -1724,8 +2087,20 @@
       <c r="J23">
         <v>100000</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23" s="5">
+        <f t="shared" si="1"/>
+        <v>38273.684632497687</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="2"/>
+        <v>29274.187085517504</v>
+      </c>
+      <c r="M23">
+        <f>(G23/J23)*Sheet1!$B$2</f>
+        <v>5.3900814643810982E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1.8333333333333299</v>
       </c>
@@ -1756,8 +2131,20 @@
       <c r="J24">
         <v>100000</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24" s="5">
+        <f t="shared" si="1"/>
+        <v>38276.871696734765</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="2"/>
+        <v>29293.123110123714</v>
+      </c>
+      <c r="M24">
+        <f>(G24/J24)*Sheet1!$B$2</f>
+        <v>5.1084519535239883E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1.9166666666666601</v>
       </c>
@@ -1788,8 +2175,20 @@
       <c r="J25">
         <v>100000</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25" s="5">
+        <f t="shared" si="1"/>
+        <v>38279.887952101439</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="2"/>
+        <v>29306.39713390607</v>
+      </c>
+      <c r="M25">
+        <f>(G25/J25)*Sheet1!$B$2</f>
+        <v>4.8471354837413315E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1820,8 +2219,20 @@
       <c r="J26">
         <v>100000</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26" s="5">
+        <f t="shared" si="1"/>
+        <v>38282.74562797416</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="2"/>
+        <v>29315.191714285767</v>
+      </c>
+      <c r="M26">
+        <f>(G26/J26)*Sheet1!$B$2</f>
+        <v>4.6047283850124159E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2.0833333333333299</v>
       </c>
@@ -1852,8 +2263,20 @@
       <c r="J27">
         <v>100000</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K27" s="5">
+        <f t="shared" si="1"/>
+        <v>38285.45608640158</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="2"/>
+        <v>29320.472547959656</v>
+      </c>
+      <c r="M27">
+        <f>(G27/J27)*Sheet1!$B$2</f>
+        <v>4.3798934821586863E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2.1666666666666599</v>
       </c>
@@ -1884,8 +2307,20 @@
       <c r="J28">
         <v>100000</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28" s="5">
+        <f t="shared" si="1"/>
+        <v>38288.029869569822</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="2"/>
+        <v>29323.026397565009</v>
+      </c>
+      <c r="M28">
+        <f>(G28/J28)*Sheet1!$B$2</f>
+        <v>4.1713659576466549E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2.25</v>
       </c>
@@ -1916,8 +2351,20 @@
       <c r="J29">
         <v>100000</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29" s="5">
+        <f t="shared" si="1"/>
+        <v>38290.476748981746</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="2"/>
+        <v>29323.492498474501</v>
+      </c>
+      <c r="M29">
+        <f>(G29/J29)*Sheet1!$B$2</f>
+        <v>3.9779561547921098E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2.3333333333333299</v>
       </c>
@@ -1948,8 +2395,20 @@
       <c r="J30">
         <v>100000</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K30" s="5">
+        <f t="shared" si="1"/>
+        <v>38292.805774845066</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="2"/>
+        <v>29322.38856764479</v>
+      </c>
+      <c r="M30">
+        <f>(G30/J30)*Sheet1!$B$2</f>
+        <v>3.7985501468750825E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2.4166666666666599</v>
       </c>
@@ -1980,8 +2439,20 @@
       <c r="J31">
         <v>100000</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K31" s="5">
+        <f t="shared" si="1"/>
+        <v>38295.025324674127</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="2"/>
+        <v>29320.132331992118</v>
+      </c>
+      <c r="M31">
+        <f>(G31/J31)*Sheet1!$B$2</f>
+        <v>3.6321086830160236E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2.5</v>
       </c>
@@ -2012,8 +2483,20 @@
       <c r="J32">
         <v>100000</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K32" s="5">
+        <f t="shared" si="1"/>
+        <v>38297.143150406104</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="2"/>
+        <v>29317.059339533371</v>
+      </c>
+      <c r="M32">
+        <f>(G32/J32)*Sheet1!$B$2</f>
+        <v>3.4776649843440243E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2.5833333333333299</v>
       </c>
@@ -2044,8 +2527,20 @@
       <c r="J33">
         <v>100000</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K33" s="5">
+        <f t="shared" si="1"/>
+        <v>38299.16642352497</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="2"/>
+        <v>29313.437690398496</v>
+      </c>
+      <c r="M33">
+        <f>(G33/J33)*Sheet1!$B$2</f>
+        <v>3.3343217655380016E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2.6666666666666599</v>
       </c>
@@ -2076,8 +2571,20 @@
       <c r="J34">
         <v>100000</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K34" s="5">
+        <f t="shared" si="1"/>
+        <v>38301.1017778979</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="2"/>
+        <v>29309.480212878694</v>
+      </c>
+      <c r="M34">
+        <f>(G34/J34)*Sheet1!$B$2</f>
+        <v>3.2012477577059724E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2.75</v>
       </c>
@@ -2108,8 +2615,20 @@
       <c r="J35">
         <v>100000</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K35" s="5">
+        <f t="shared" si="1"/>
+        <v>38302.955350147837</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="2"/>
+        <v>29305.354522286972</v>
+      </c>
+      <c r="M35">
+        <f>(G35/J35)*Sheet1!$B$2</f>
+        <v>3.0776739456897927E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2.8333333333333299</v>
       </c>
@@ -2140,8 +2659,20 @@
       <c r="J36">
         <v>100000</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K36" s="5">
+        <f t="shared" si="1"/>
+        <v>38304.732817482836</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="2"/>
+        <v>29301.191325507836</v>
+      </c>
+      <c r="M36">
+        <f>(G36/J36)*Sheet1!$B$2</f>
+        <v>2.9628896779422536E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2.9166666666666599</v>
       </c>
@@ -2172,8 +2703,20 @@
       <c r="J37">
         <v>100000</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K37" s="5">
+        <f t="shared" si="1"/>
+        <v>38306.43943298528</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="2"/>
+        <v>29297.09127200078</v>
+      </c>
+      <c r="M37">
+        <f>(G37/J37)*Sheet1!$B$2</f>
+        <v>2.8562387637699658E-5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2204,8 +2747,20 @@
       <c r="J38">
         <v>100000</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K38" s="5">
+        <f t="shared" si="1"/>
+        <v>38308.080058406435</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="2"/>
+        <v>29293.130601200559</v>
+      </c>
+      <c r="M38">
+        <f>(G38/J38)*Sheet1!$B$2</f>
+        <v>2.7571156415630662E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3.0833333333333299</v>
       </c>
@@ -2236,8 +2791,20 @@
       <c r="J39">
         <v>100000</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K39" s="5">
+        <f t="shared" si="1"/>
+        <v>38309.659194555083</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="2"/>
+        <v>29289.365793386296</v>
+      </c>
+      <c r="M39">
+        <f>(G39/J39)*Sheet1!$B$2</f>
+        <v>2.6649616755945111E-5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3.1666666666666599</v>
       </c>
@@ -2268,8 +2835,20 @@
       <c r="J40">
         <v>100000</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K40" s="5">
+        <f t="shared" si="1"/>
+        <v>38311.181009389846</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="2"/>
+        <v>29285.837395832699</v>
+      </c>
+      <c r="M40">
+        <f>(G40/J40)*Sheet1!$B$2</f>
+        <v>2.5792616199202154E-5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3.25</v>
       </c>
@@ -2300,8 +2879,20 @@
       <c r="J41">
         <v>100000</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K41" s="5">
+        <f t="shared" si="1"/>
+        <v>38312.649363939759</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="2"/>
+        <v>29282.573166738035</v>
+      </c>
+      <c r="M41">
+        <f>(G41/J41)*Sheet1!$B$2</f>
+        <v>2.4995402734133074E-5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3.3333333333333299</v>
       </c>
@@ -2332,8 +2923,20 @@
       <c r="J42">
         <v>100000</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K42" s="5">
+        <f t="shared" si="1"/>
+        <v>38314.067836188602</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="2"/>
+        <v>29279.590655289114</v>
+      </c>
+      <c r="M42">
+        <f>(G42/J42)*Sheet1!$B$2</f>
+        <v>2.4253593386992069E-5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3.4166666666666599</v>
       </c>
@@ -2364,8 +2967,20 @@
       <c r="J43">
         <v>100000</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K43" s="5">
+        <f t="shared" si="1"/>
+        <v>38315.439743051138</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="2"/>
+        <v>29276.899313942562</v>
+      </c>
+      <c r="M43">
+        <f>(G43/J43)*Sheet1!$B$2</f>
+        <v>2.3563144908056022E-5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>3.5</v>
       </c>
@@ -2396,8 +3011,20 @@
       <c r="J44">
         <v>100000</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K44" s="5">
+        <f t="shared" si="1"/>
+        <v>38316.768160598571</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="2"/>
+        <v>29274.50223010268</v>
+      </c>
+      <c r="M44">
+        <f>(G44/J44)*Sheet1!$B$2</f>
+        <v>2.2920326520818078E-5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>3.5833333333333299</v>
       </c>
@@ -2428,8 +3055,20 @@
       <c r="J45">
         <v>100000</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K45" s="5">
+        <f t="shared" si="1"/>
+        <v>38318.055942612722</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="2"/>
+        <v>29272.397528930425</v>
+      </c>
+      <c r="M45">
+        <f>(G45/J45)*Sheet1!$B$2</f>
+        <v>2.2321694734762772E-5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>3.6666666666666599</v>
       </c>
@@ -2460,8 +3099,20 @@
       <c r="J46">
         <v>100000</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K46" s="5">
+        <f t="shared" si="1"/>
+        <v>38319.305737709306</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="2"/>
+        <v>29270.579535309505</v>
+      </c>
+      <c r="M46">
+        <f>(G46/J46)*Sheet1!$B$2</f>
+        <v>2.1764070027578876E-5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>3.75</v>
       </c>
@@ -2492,8 +3143,20 @@
       <c r="J47">
         <v>100000</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K47" s="5">
+        <f t="shared" si="1"/>
+        <v>38320.520004989754</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="2"/>
+        <v>29269.039697014316</v>
+      </c>
+      <c r="M47">
+        <f>(G47/J47)*Sheet1!$B$2</f>
+        <v>2.1244515461319135E-5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>3.8333333333333299</v>
       </c>
@@ -2524,8 +3187,20 @@
       <c r="J48">
         <v>100000</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K48" s="5">
+        <f t="shared" si="1"/>
+        <v>38321.701028445132</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="2"/>
+        <v>29267.767337551701</v>
+      </c>
+      <c r="M48">
+        <f>(G48/J48)*Sheet1!$B$2</f>
+        <v>2.0760317011245441E-5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>3.9166666666666599</v>
       </c>
@@ -2556,8 +3231,20 @@
       <c r="J49">
         <v>100000</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K49" s="5">
+        <f t="shared" si="1"/>
+        <v>38322.850930204942</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="2"/>
+        <v>29266.750268622833</v>
+      </c>
+      <c r="M49">
+        <f>(G49/J49)*Sheet1!$B$2</f>
+        <v>2.0308965511905055E-5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>4</v>
       </c>
@@ -2588,8 +3275,20 @@
       <c r="J50">
         <v>100000</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K50" s="5">
+        <f t="shared" si="1"/>
+        <v>38323.971682706484</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="2"/>
+        <v>29265.975276862402</v>
+      </c>
+      <c r="M50">
+        <f>(G50/J50)*Sheet1!$B$2</f>
+        <v>1.9888140107991337E-5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>4.0833333333333304</v>
       </c>
@@ -2620,8 +3319,20 @@
       <c r="J51">
         <v>100000</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K51" s="5">
+        <f t="shared" si="1"/>
+        <v>38325.065119882827</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="2"/>
+        <v>29265.428513206487</v>
+      </c>
+      <c r="M51">
+        <f>(G51/J51)*Sheet1!$B$2</f>
+        <v>1.9495693105293047E-5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>4.1666666666666599</v>
       </c>
@@ -2652,8 +3363,20 @@
       <c r="J52">
         <v>100000</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K52" s="5">
+        <f t="shared" si="1"/>
+        <v>38326.132947452679</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="2"/>
+        <v>29265.095801643729</v>
+      </c>
+      <c r="M52">
+        <f>(G52/J52)*Sheet1!$B$2</f>
+        <v>1.9129636107719849E-5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>4.25</v>
       </c>
@@ -2684,8 +3407,20 @@
       <c r="J53">
         <v>100000</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K53" s="5">
+        <f t="shared" si="1"/>
+        <v>38327.176752388987</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="2"/>
+        <v>29264.962881555537</v>
+      </c>
+      <c r="M53">
+        <f>(G53/J53)*Sheet1!$B$2</f>
+        <v>1.8788127330700956E-5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>4.3333333333333304</v>
       </c>
@@ -2716,8 +3451,20 @@
       <c r="J54">
         <v>100000</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K54" s="5">
+        <f t="shared" si="1"/>
+        <v>38328.198011636821</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="2"/>
+        <v>29265.015596394136</v>
+      </c>
+      <c r="M54">
+        <f>(G54/J54)*Sheet1!$B$2</f>
+        <v>1.8469459996257951E-5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>4.4166666666666599</v>
       </c>
@@ -2748,8 +3495,20 @@
       <c r="J55">
         <v>100000</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K55" s="5">
+        <f t="shared" si="1"/>
+        <v>38329.198100143556</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="2"/>
+        <v>29265.240038454125</v>
+      </c>
+      <c r="M55">
+        <f>(G55/J55)*Sheet1!$B$2</f>
+        <v>1.8172051715026289E-5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>4.5</v>
       </c>
@@ -2780,8 +3539,20 @@
       <c r="J56">
         <v>100000</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K56" s="5">
+        <f t="shared" si="1"/>
+        <v>38330.178298260922</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="2"/>
+        <v>29265.622658030654</v>
+      </c>
+      <c r="M56">
+        <f>(G56/J56)*Sheet1!$B$2</f>
+        <v>1.7894434769247329E-5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>4.5833333333333304</v>
       </c>
@@ -2812,8 +3583,20 @@
       <c r="J57">
         <v>100000</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K57" s="5">
+        <f t="shared" si="1"/>
+        <v>38331.139798570606</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="2"/>
+        <v>29266.150343803893</v>
+      </c>
+      <c r="M57">
+        <f>(G57/J57)*Sheet1!$B$2</f>
+        <v>1.7635247217763506E-5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>4.6666666666666599</v>
       </c>
@@ -2844,8 +3627,20 @@
       <c r="J58">
         <v>100000</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K58" s="5">
+        <f t="shared" si="1"/>
+        <v>38332.0837121847</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="2"/>
+        <v>29266.81048001282</v>
+      </c>
+      <c r="M58">
+        <f>(G58/J58)*Sheet1!$B$2</f>
+        <v>1.7393224749606903E-5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>4.75</v>
       </c>
@@ -2876,8 +3671,20 @@
       <c r="J59">
         <v>100000</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K59" s="5">
+        <f t="shared" si="1"/>
+        <v>38333.011074561444</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="2"/>
+        <v>29267.59098502067</v>
+      </c>
+      <c r="M59">
+        <f>(G59/J59)*Sheet1!$B$2</f>
+        <v>1.7167193219413292E-5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>4.8333333333333304</v>
       </c>
@@ -2908,8 +3715,20 @@
       <c r="J60">
         <v>100000</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K60" s="5">
+        <f t="shared" si="1"/>
+        <v>38333.922850880379</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="2"/>
+        <v>29268.480335041884</v>
+      </c>
+      <c r="M60">
+        <f>(G60/J60)*Sheet1!$B$2</f>
+        <v>1.6956061803593329E-5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>4.9166666666666599</v>
       </c>
@@ -2940,8 +3759,20 @@
       <c r="J61">
         <v>100000</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K61" s="5">
+        <f t="shared" si="1"/>
+        <v>38334.81994101045</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="2"/>
+        <v>29269.46757611242</v>
+      </c>
+      <c r="M61">
+        <f>(G61/J61)*Sheet1!$B$2</f>
+        <v>1.6758816721583675E-5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>5</v>
       </c>
@@ -2971,9 +3802,266 @@
       </c>
       <c r="J62">
         <v>100000</v>
+      </c>
+      <c r="K62" s="5">
+        <f t="shared" si="1"/>
+        <v>38335.7031841063</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="2"/>
+        <v>29270.542326825522</v>
+      </c>
+      <c r="M62">
+        <f>(G62/J62)*Sheet1!$B$2</f>
+        <v>1.6574515471609825E-5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>6.0439999999999999E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>0.38295656500000003</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0.30471698899999999</v>
+      </c>
+      <c r="E11">
+        <v>0.30471698899999999</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>7.6094580000000004E-3</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E12">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>3.3402220000000003E-2</v>
+      </c>
+      <c r="C13">
+        <v>3.3402220000000003E-2</v>
+      </c>
+      <c r="D13">
+        <v>3.3402220000000003E-2</v>
+      </c>
+      <c r="E13">
+        <v>3.3402220000000003E-2</v>
+      </c>
+      <c r="F13">
+        <v>3.3402220000000003E-2</v>
+      </c>
+      <c r="G13">
+        <v>0.15222221999999999</v>
+      </c>
+      <c r="H13">
+        <v>3.3402220000000003E-2</v>
+      </c>
+      <c r="I13">
+        <v>3.3402220000000003E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>3.3153780000000001E-2</v>
+      </c>
+      <c r="C14">
+        <v>3.3153780000000001E-2</v>
+      </c>
+      <c r="D14">
+        <v>3.3153780000000001E-2</v>
+      </c>
+      <c r="E14">
+        <v>3.3153780000000001E-2</v>
+      </c>
+      <c r="F14">
+        <v>3.3153780000000001E-2</v>
+      </c>
+      <c r="G14">
+        <v>0.14933332999999999</v>
+      </c>
+      <c r="H14">
+        <v>3.3153780000000001E-2</v>
+      </c>
+      <c r="I14">
+        <v>3.3153700000000001E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1">
+        <v>0.222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3">
+        <f>B1*B2</f>
+        <v>1.7760000000000001E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>